<commit_message>
Improve parser tests with incorrectly formatted files
</commit_message>
<xml_diff>
--- a/server/test/csv_parser/files/bad_formatted_files/invalid_column.xlsx
+++ b/server/test/csv_parser/files/bad_formatted_files/invalid_column.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\ParserTests\CSVFiles\WrongFormattedFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\csv_parser\files\bad_formatted_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBEE501-D2A3-417E-8732-C52E87DE5D86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B2A849-F4BC-454E-9187-DEC58C88921F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1380,13 +1380,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="18.33203125" style="4" customWidth="1"/>
     <col min="4" max="5" width="33.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" customWidth="1"/>
     <col min="7" max="7" width="34.109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" style="2" customWidth="1"/>

</xml_diff>